<commit_message>
Error images displayed on the front end. Bugs fixed while generating word document
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy-1.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Address</t>
   </si>
@@ -22,56 +22,76 @@
     <t>Country</t>
   </si>
   <si>
-    <t>Sub Investigator</t>
-  </si>
-  <si>
-    <t>PI Name</t>
-  </si>
-  <si>
-    <t>PI Medical license #</t>
-  </si>
-  <si>
     <t>Institute Name</t>
   </si>
   <si>
-    <t>Sub Investigator ML#</t>
-  </si>
-  <si>
-    <t>SI Qualification</t>
-  </si>
-  <si>
-    <t>PI Qualification</t>
-  </si>
-  <si>
     <t>Project Number</t>
   </si>
   <si>
-    <t>Sponsor Protocol #</t>
+    <t>Investigator Name</t>
+  </si>
+  <si>
+    <t>Medical license Number</t>
+  </si>
+  <si>
+    <t>Qualification</t>
+  </si>
+  <si>
+    <t>Sponsor Protocol Number</t>
+  </si>
+  <si>
+    <t>Role (Principal/Sub)</t>
+  </si>
+  <si>
+    <t>Principal</t>
   </si>
   <si>
     <t>MD</t>
   </si>
   <si>
+    <t>Sub</t>
+  </si>
+  <si>
+    <t>0102/0304</t>
+  </si>
+  <si>
+    <t>DeLuca Jr., William F</t>
+  </si>
+  <si>
     <t>#6789</t>
   </si>
   <si>
-    <t>AA44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cleveland USA
-</t>
+    <t xml:space="preserve">brown, malcolm d </t>
   </si>
   <si>
     <t>#11667</t>
   </si>
   <si>
-    <t>0102/0304</t>
+    <t>David C. Kauffman</t>
+  </si>
+  <si>
+    <t>Liang, Cheng Yi</t>
+  </si>
+  <si>
+    <t>MARTIN S MOK</t>
+  </si>
+  <si>
+    <t>#859015</t>
   </si>
   <si>
     <t>0506/0708</t>
   </si>
   <si>
-    <t>#859015</t>
+    <t xml:space="preserve">Jolly, Jr., Henry W., </t>
+  </si>
+  <si>
+    <t>Xing H. Rosie</t>
+  </si>
+  <si>
+    <t>VAN DER HEIJDE, DESIREE</t>
+  </si>
+  <si>
+    <t>MAYER JANE MARIE</t>
   </si>
   <si>
     <t>#89277</t>
@@ -81,36 +101,6 @@
   </si>
   <si>
     <t>0910/1112</t>
-  </si>
-  <si>
-    <t>Delhi, India</t>
-  </si>
-  <si>
-    <t>David C. Kauffman</t>
-  </si>
-  <si>
-    <t>DeLuca Jr., William F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brown, malcolm d </t>
-  </si>
-  <si>
-    <t>Liang, Cheng Yi</t>
-  </si>
-  <si>
-    <t>MARTIN S MOK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jolly, Jr., Henry W., </t>
-  </si>
-  <si>
-    <t>Xing H. Rosie</t>
-  </si>
-  <si>
-    <t>VAN DER HEIJDE, DESIREE</t>
-  </si>
-  <si>
-    <t>MAYER JANE MARIE</t>
   </si>
   <si>
     <t>Choudry, Mubashar</t>
@@ -126,7 +116,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +131,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -178,16 +180,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,221 +501,357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:BF14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="26" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="2"/>
+    </row>
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+    </row>
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>